<commit_message>
Add MONTH function description
</commit_message>
<xml_diff>
--- a/xlsx/tests/docs/MONTH.xlsx
+++ b/xlsx/tests/docs/MONTH.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\IronCalc work\Function descriptions\Date and Time\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\IronCalc work\IronCalc-clone\IronCalc-SF\xlsx\tests\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A79784E-10B1-4AC5-83EF-9061582B1259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F9EB9C-1F9C-435F-B656-8076131F3C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C7E191B1-44A3-4478-A86F-CB5CE7E3580C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Comments</t>
   </si>
@@ -47,22 +47,58 @@
     <t>Using DATE function</t>
   </si>
   <si>
-    <t>Date literal</t>
-  </si>
-  <si>
     <t>Integer serial number</t>
   </si>
   <si>
     <t>Serial number with fractional part</t>
   </si>
   <si>
+    <t>Formula Text</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Largest accepted serial number</t>
+  </si>
+  <si>
+    <t>Smallest accepted serial number</t>
+  </si>
+  <si>
+    <t>Excel considers this 29/02/1900 (although 1900 was not a leap year)</t>
+  </si>
+  <si>
+    <t>Example of error propagation</t>
+  </si>
+  <si>
+    <t>Unable to convert date argument to a number</t>
+  </si>
+  <si>
+    <t>Negative serial number</t>
+  </si>
+  <si>
+    <t>Serial number too large</t>
+  </si>
+  <si>
+    <t>Input causes a #DIV/0! error</t>
+  </si>
+  <si>
     <t>MONTH()</t>
+  </si>
+  <si>
+    <t>Zero serial number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -80,12 +116,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -100,13 +142,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,79 +503,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6100931E-B86C-4134-94C5-0A5BD3A5B1E4}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>45619</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="6">
+        <v>45651</v>
+      </c>
+      <c r="B2" s="2">
         <f>MONTH(A2)</f>
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B2)</f>
+        <v>=MONTH(A2)</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <f>MONTH(DATE(2024, 11, 23))</f>
-        <v>11</v>
+      <c r="A3" s="7"/>
+      <c r="B3" s="2">
+        <f>MONTH(DATE(2024,12,25))</f>
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="str">
+        <f t="shared" ref="C3:C10" ca="1" si="0">_xlfn.FORMULATEXT(B3)</f>
+        <v>=MONTH(DATE(2024,12,25))</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <f>MONTH("2024-11-23")</f>
-        <v>11</v>
+      <c r="A4" s="2">
+        <v>45651</v>
+      </c>
+      <c r="B4" s="2">
+        <f>MONTH(A4)</f>
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=MONTH(A4)</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>45619</v>
-      </c>
-      <c r="B5">
+      <c r="A5" s="2">
+        <v>45651.9</v>
+      </c>
+      <c r="B5" s="2">
         <f>MONTH(A5)</f>
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=MONTH(A5)</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>45619.9</v>
-      </c>
-      <c r="B6">
-        <f>MONTH(A6)</f>
+      <c r="A6" s="2"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <f>MONTH(A7)</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B7)</f>
+        <v>=MONTH(A7)</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2">
+        <f>MONTH(A8)</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B8)</f>
+        <v>=MONTH(A8)</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>46016</v>
+      </c>
+      <c r="B9" s="2">
+        <f>MONTH(A9)</f>
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B9)</f>
+        <v>=MONTH(A9)</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>2958465.999988426</v>
+      </c>
+      <c r="B10" s="2">
+        <f>MONTH(A10)</f>
+        <v>12</v>
+      </c>
+      <c r="C10" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=MONTH(A10)</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+    </row>
+    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="e">
+        <f>MONTH(SQRT(-1))</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="B14" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A14)</f>
+        <v>=MONTH(SQRT(-1))</v>
+      </c>
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
-        <v>5</v>
+    </row>
+    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="e">
+        <f>MONTH("str")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B15" s="3" t="str">
+        <f t="shared" ref="B15:B16" ca="1" si="1">_xlfn.FORMULATEXT(A15)</f>
+        <v>=MONTH("str")</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="e">
+        <f>MONTH(10/0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="B16" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=MONTH(10/0)</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="e">
+        <f>MONTH(-5)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="B17" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A17)</f>
+        <v>=MONTH(-5)</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <f>MONTH(0)</f>
+        <v>1</v>
+      </c>
+      <c r="B18" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A18)</f>
+        <v>=MONTH(0)</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="e">
+        <f>MONTH(2958466)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="B19" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A19)</f>
+        <v>=MONTH(2958466)</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <f>MONTH(DATE(1900,2,29))</f>
+        <v>2</v>
+      </c>
+      <c r="B20" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A20)</f>
+        <v>=MONTH(DATE(1900,2,29))</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>